<commit_message>
Update novembro e outubro
</commit_message>
<xml_diff>
--- a/GestorReceitas/outubro/relatorioMensal_outubro.xlsx
+++ b/GestorReceitas/outubro/relatorioMensal_outubro.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\pessoal\AssociacaodePais\School\GestorReceitas\Outubro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A04301B-B672-44DE-947A-2A8E8B22D48D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EE332D5-15B1-46E9-AE46-FFBF1F50B356}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15690" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="relatorioMensal" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="455">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="456">
   <si>
     <t>Nome</t>
   </si>
@@ -674,9 +674,6 @@
     <t>289182573</t>
   </si>
   <si>
-    <t>Lanche de Setembro + outubro</t>
-  </si>
-  <si>
     <t>tania.cabeleireira.87@gmail.com</t>
   </si>
   <si>
@@ -1404,6 +1401,12 @@
   </si>
   <si>
     <t>328390628</t>
+  </si>
+  <si>
+    <t>Tirar Recibo Lanche de Setembro + outubro</t>
+  </si>
+  <si>
+    <t>Confirmar prolongamentos para afonso monteiro ferreira</t>
   </si>
 </sst>
 </file>
@@ -1413,7 +1416,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;€ &quot;#,##0.00"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1425,25 +1428,43 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1486,6 +1507,12 @@
         <bgColor rgb="FF00FFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FF00"/>
+        <bgColor rgb="FFFF0000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -1521,7 +1548,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1541,7 +1568,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="2" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1549,6 +1575,15 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3151,6 +3186,11 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF00FF00"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -3363,20 +3403,19 @@
   <dimension ref="A1:Q1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M100" sqref="M100"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="42" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="2.85546875" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" hidden="1" customWidth="1"/>
-    <col min="5" max="6" width="3.28515625" hidden="1" customWidth="1"/>
-    <col min="7" max="10" width="12.28515625" hidden="1" customWidth="1"/>
-    <col min="11" max="15" width="12.28515625" customWidth="1"/>
-    <col min="16" max="16" width="29.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="2.85546875" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" customWidth="1"/>
+    <col min="5" max="6" width="3.28515625" customWidth="1"/>
+    <col min="7" max="15" width="12.28515625" customWidth="1"/>
+    <col min="16" max="16" width="38.85546875" customWidth="1"/>
     <col min="17" max="17" width="36.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3480,7 +3519,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>22</v>
       </c>
@@ -3519,6 +3558,9 @@
         <f t="shared" si="0"/>
         <v>-10</v>
       </c>
+      <c r="P3" s="26" t="s">
+        <v>455</v>
+      </c>
       <c r="Q3" s="3" t="s">
         <v>25</v>
       </c>
@@ -3680,7 +3722,7 @@
       </c>
     </row>
     <row r="7" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="22" t="s">
         <v>39</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -3712,15 +3754,15 @@
         <v>0</v>
       </c>
       <c r="L7" s="4">
-        <f>20-4</f>
-        <v>16</v>
+        <f>20-4+11</f>
+        <v>27</v>
       </c>
       <c r="M7" s="5">
         <v>0</v>
       </c>
       <c r="N7" s="5">
         <f>L7 + K7   +  M7 - (G7 + H7 + I7 +J7)+3</f>
-        <v>-11</v>
+        <v>0</v>
       </c>
       <c r="Q7" s="3" t="s">
         <v>41</v>
@@ -3802,6 +3844,7 @@
         <v>0</v>
       </c>
       <c r="L9" s="4">
+        <f>45-0.5</f>
         <v>44.5</v>
       </c>
       <c r="M9" s="5">
@@ -3865,7 +3908,7 @@
       </c>
     </row>
     <row r="11" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="22" t="s">
         <v>54</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -3897,14 +3940,14 @@
         <v>0</v>
       </c>
       <c r="L11" s="4">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="M11" s="5">
         <v>0</v>
       </c>
       <c r="N11" s="5">
         <f t="shared" si="1"/>
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="Q11" s="3" t="s">
         <v>57</v>
@@ -4009,7 +4052,7 @@
       </c>
     </row>
     <row r="14" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="22" t="s">
         <v>64</v>
       </c>
       <c r="B14" s="3" t="s">
@@ -4041,15 +4084,15 @@
         <v>0</v>
       </c>
       <c r="L14" s="4">
-        <f>-6+35</f>
-        <v>29</v>
+        <f>-6+35+11</f>
+        <v>40</v>
       </c>
       <c r="M14" s="5">
         <v>0</v>
       </c>
       <c r="N14" s="5">
         <f>L14 + K14   +  M14 - (G14 + H14 + I14 +J14)+5</f>
-        <v>-11</v>
+        <v>0</v>
       </c>
       <c r="Q14" s="3" t="s">
         <v>41</v>
@@ -4444,7 +4487,7 @@
       </c>
     </row>
     <row r="23" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="22" t="s">
         <v>90</v>
       </c>
       <c r="B23" s="3" t="s">
@@ -4478,15 +4521,15 @@
         <v>0</v>
       </c>
       <c r="L23" s="4">
-        <f>92.5-24.5</f>
-        <v>68</v>
+        <f>92.5-24.5+6</f>
+        <v>74</v>
       </c>
       <c r="M23" s="5">
         <v>0</v>
       </c>
       <c r="N23" s="5">
         <f t="shared" si="2"/>
-        <v>-6</v>
+        <v>0</v>
       </c>
       <c r="Q23" s="3" t="s">
         <v>92</v>
@@ -4934,7 +4977,7 @@
       </c>
     </row>
     <row r="33" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="7" t="s">
+      <c r="A33" s="22" t="s">
         <v>119</v>
       </c>
       <c r="B33" s="3" t="s">
@@ -4977,7 +5020,7 @@
       </c>
     </row>
     <row r="34" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="7" t="s">
+      <c r="A34" s="22" t="s">
         <v>122</v>
       </c>
       <c r="B34" s="3" t="s">
@@ -5058,6 +5101,7 @@
         <f t="shared" si="2"/>
         <v>-45</v>
       </c>
+      <c r="O35" s="24"/>
       <c r="Q35" s="3" t="s">
         <v>127</v>
       </c>
@@ -5196,6 +5240,7 @@
         <f t="shared" si="2"/>
         <v>-67.5</v>
       </c>
+      <c r="O38" s="24"/>
       <c r="Q38" s="3" t="s">
         <v>136</v>
       </c>
@@ -5587,6 +5632,7 @@
         <f t="shared" si="2"/>
         <v>-4</v>
       </c>
+      <c r="O46" s="24"/>
       <c r="Q46" s="3" t="s">
         <v>160</v>
       </c>
@@ -5695,7 +5741,7 @@
       </c>
     </row>
     <row r="49" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="7" t="s">
+      <c r="A49" s="22" t="s">
         <v>168</v>
       </c>
       <c r="B49" s="3" t="s">
@@ -5793,7 +5839,7 @@
       </c>
     </row>
     <row r="51" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="7" t="s">
+      <c r="A51" s="22" t="s">
         <v>175</v>
       </c>
       <c r="B51" s="3" t="s">
@@ -5827,14 +5873,15 @@
         <v>0</v>
       </c>
       <c r="L51" s="4">
-        <v>25</v>
+        <f>50+25</f>
+        <v>75</v>
       </c>
       <c r="M51" s="5">
         <v>0</v>
       </c>
       <c r="N51" s="5">
         <f t="shared" si="2"/>
-        <v>-50</v>
+        <v>0</v>
       </c>
       <c r="Q51" s="3" t="s">
         <v>177</v>
@@ -6251,7 +6298,7 @@
       </c>
     </row>
     <row r="60" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="7" t="s">
+      <c r="A60" s="22" t="s">
         <v>202</v>
       </c>
       <c r="B60" s="3" t="s">
@@ -6283,14 +6330,14 @@
         <v>0</v>
       </c>
       <c r="L60" s="4">
-        <v>0</v>
+        <v>57</v>
       </c>
       <c r="M60" s="5">
         <v>0</v>
       </c>
       <c r="N60" s="5">
         <f t="shared" si="2"/>
-        <v>-57</v>
+        <v>0</v>
       </c>
       <c r="Q60" s="3" t="s">
         <v>204</v>
@@ -6350,8 +6397,8 @@
         <v>208</v>
       </c>
     </row>
-    <row r="62" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="7" t="s">
+    <row r="62" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A62" s="22" t="s">
         <v>209</v>
       </c>
       <c r="B62" s="3" t="s">
@@ -6384,26 +6431,26 @@
         <v>0</v>
       </c>
       <c r="L62" s="4">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="M62" s="5">
         <v>7.5</v>
       </c>
       <c r="N62" s="5">
         <f t="shared" si="2"/>
-        <v>-19</v>
+        <v>0</v>
       </c>
       <c r="O62" s="13"/>
-      <c r="P62" s="17" t="s">
+      <c r="P62" s="25" t="s">
+        <v>454</v>
+      </c>
+      <c r="Q62" s="3" t="s">
         <v>211</v>
-      </c>
-      <c r="Q62" s="3" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="63" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>23</v>
@@ -6412,7 +6459,7 @@
         <v>1</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E63" s="3">
         <v>0</v>
@@ -6449,12 +6496,12 @@
         <v>20</v>
       </c>
       <c r="Q63" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="64" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>55</v>
@@ -6463,7 +6510,7 @@
         <v>1</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E64" s="3">
         <v>0</v>
@@ -6500,12 +6547,12 @@
         <v>20</v>
       </c>
       <c r="Q64" s="3" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
         <v>218</v>
-      </c>
-    </row>
-    <row r="65" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="2" t="s">
-        <v>219</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>23</v>
@@ -6514,7 +6561,7 @@
         <v>1</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E65" s="3">
         <v>20</v>
@@ -6528,7 +6575,7 @@
       <c r="H65" s="4">
         <v>0</v>
       </c>
-      <c r="I65" s="18" t="s">
+      <c r="I65" s="17" t="s">
         <v>19</v>
       </c>
       <c r="J65" s="4"/>
@@ -6556,8 +6603,8 @@
       </c>
     </row>
     <row r="66" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="7" t="s">
-        <v>221</v>
+      <c r="A66" s="22" t="s">
+        <v>220</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>51</v>
@@ -6566,7 +6613,7 @@
         <v>1</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E66" s="3">
         <v>0</v>
@@ -6590,23 +6637,23 @@
         <v>0</v>
       </c>
       <c r="L66" s="4">
-        <f>32.5-7.5</f>
-        <v>25</v>
+        <f>32.5-7.5+15</f>
+        <v>40</v>
       </c>
       <c r="M66" s="5">
         <v>0</v>
       </c>
       <c r="N66" s="5">
         <f t="shared" si="2"/>
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="Q66" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="67" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>55</v>
@@ -6615,7 +6662,7 @@
         <v>1</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E67" s="3">
         <v>0</v>
@@ -6650,12 +6697,12 @@
         <v>45</v>
       </c>
       <c r="Q67" s="3" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
         <v>226</v>
-      </c>
-    </row>
-    <row r="68" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="2" t="s">
-        <v>227</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>17</v>
@@ -6664,7 +6711,7 @@
         <v>1</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E68" s="3">
         <v>0</v>
@@ -6699,12 +6746,12 @@
         <v>20</v>
       </c>
       <c r="Q68" s="3" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="22" t="s">
         <v>229</v>
-      </c>
-    </row>
-    <row r="69" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="7" t="s">
-        <v>230</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>23</v>
@@ -6713,7 +6760,7 @@
         <v>1</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E69" s="3">
         <v>22</v>
@@ -6737,23 +6784,23 @@
         <v>0</v>
       </c>
       <c r="L69" s="4">
-        <f>-22.5+47.5</f>
-        <v>25</v>
+        <f>-22.5+47.5+49</f>
+        <v>74</v>
       </c>
       <c r="M69" s="5">
         <v>0</v>
       </c>
       <c r="N69" s="5">
         <f t="shared" si="2"/>
-        <v>-49</v>
+        <v>0</v>
       </c>
       <c r="Q69" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="70" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>31</v>
@@ -6762,7 +6809,7 @@
         <v>1</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E70" s="3">
         <v>0</v>
@@ -6797,18 +6844,18 @@
         <v>20</v>
       </c>
       <c r="Q70" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="71" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B71" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E71" s="3">
         <v>22</v>
@@ -6839,13 +6886,14 @@
         <f t="shared" si="2"/>
         <v>-73.5</v>
       </c>
+      <c r="O71" s="24"/>
       <c r="Q71" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="72" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>23</v>
@@ -6854,7 +6902,7 @@
         <v>1</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E72" s="3">
         <v>23</v>
@@ -6868,7 +6916,7 @@
       <c r="H72" s="4">
         <v>0</v>
       </c>
-      <c r="I72" s="18" t="s">
+      <c r="I72" s="17" t="s">
         <v>19</v>
       </c>
       <c r="J72" s="4"/>
@@ -6889,18 +6937,18 @@
         <v>20</v>
       </c>
       <c r="Q72" s="3" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="73" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="22" t="s">
         <v>241</v>
-      </c>
-    </row>
-    <row r="73" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="7" t="s">
-        <v>242</v>
       </c>
       <c r="B73" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E73" s="3">
         <v>0</v>
@@ -6922,28 +6970,28 @@
         <v>0</v>
       </c>
       <c r="L73" s="4">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="M73" s="5">
         <v>0</v>
       </c>
       <c r="N73" s="5">
         <f t="shared" si="2"/>
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="Q73" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="74" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="7" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E74" s="3">
         <v>0</v>
@@ -6975,12 +7023,12 @@
         <v>-22.5</v>
       </c>
       <c r="Q74" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="75" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B75" s="3" t="s">
         <v>51</v>
@@ -6989,7 +7037,7 @@
         <v>1</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E75" s="3">
         <v>0</v>
@@ -7027,18 +7075,18 @@
         <v>37</v>
       </c>
       <c r="Q75" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="76" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B76" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E76" s="3">
         <v>23</v>
@@ -7069,13 +7117,14 @@
         <f t="shared" si="2"/>
         <v>-35.5</v>
       </c>
+      <c r="O76" s="24"/>
       <c r="Q76" s="3" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="77" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B77" s="3" t="s">
         <v>51</v>
@@ -7084,7 +7133,7 @@
         <v>1</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E77" s="3">
         <v>23</v>
@@ -7122,12 +7171,12 @@
         <v>20</v>
       </c>
       <c r="Q77" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="78" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B78" s="3" t="s">
         <v>27</v>
@@ -7136,7 +7185,7 @@
         <v>1</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E78" s="3">
         <v>20</v>
@@ -7144,7 +7193,7 @@
       <c r="F78" s="3">
         <v>20</v>
       </c>
-      <c r="G78" s="19">
+      <c r="G78" s="18">
         <v>39</v>
       </c>
       <c r="H78" s="4">
@@ -7172,7 +7221,7 @@
       <c r="O78" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="P78" s="20" t="s">
+      <c r="P78" s="19" t="s">
         <v>207</v>
       </c>
       <c r="Q78" s="3" t="s">
@@ -7181,13 +7230,13 @@
     </row>
     <row r="79" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B79" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E79" s="3">
         <v>0</v>
@@ -7223,12 +7272,12 @@
         <v>20</v>
       </c>
       <c r="Q79" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="80" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B80" s="3" t="s">
         <v>55</v>
@@ -7237,7 +7286,7 @@
         <v>1</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E80" s="3">
         <v>0</v>
@@ -7272,12 +7321,12 @@
         <v>20</v>
       </c>
       <c r="Q80" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="81" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B81" s="3" t="s">
         <v>55</v>
@@ -7286,7 +7335,7 @@
         <v>1</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E81" s="3">
         <v>0</v>
@@ -7321,15 +7370,15 @@
         <v>20</v>
       </c>
       <c r="P81" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="Q81" s="3" t="s">
         <v>266</v>
-      </c>
-      <c r="Q81" s="3" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="82" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B82" s="3" t="s">
         <v>23</v>
@@ -7338,7 +7387,7 @@
         <v>1</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E82" s="3">
         <v>0</v>
@@ -7352,7 +7401,7 @@
       <c r="H82" s="4">
         <v>0</v>
       </c>
-      <c r="I82" s="18" t="s">
+      <c r="I82" s="17" t="s">
         <v>19</v>
       </c>
       <c r="J82" s="4">
@@ -7376,12 +7425,12 @@
         <v>20</v>
       </c>
       <c r="Q82" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="83" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="7" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B83" s="3" t="s">
         <v>55</v>
@@ -7390,7 +7439,7 @@
         <v>1</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E83" s="3">
         <v>21</v>
@@ -7412,25 +7461,25 @@
         <v>0</v>
       </c>
       <c r="L83" s="4">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="M83" s="5">
         <v>0</v>
       </c>
       <c r="N83" s="5">
         <f t="shared" si="2"/>
-        <v>-45</v>
+        <v>0</v>
       </c>
       <c r="O83" s="6" t="s">
         <v>20</v>
       </c>
       <c r="Q83" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="84" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B84" s="3" t="s">
         <v>51</v>
@@ -7439,7 +7488,7 @@
         <v>1</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E84" s="3">
         <v>0</v>
@@ -7479,13 +7528,13 @@
     </row>
     <row r="85" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="9" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B85" s="3" t="s">
         <v>55</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E85" s="3">
         <v>0</v>
@@ -7520,18 +7569,18 @@
         <v>45</v>
       </c>
       <c r="Q85" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="86" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B86" s="3" t="s">
         <v>51</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E86" s="3">
         <v>0</v>
@@ -7566,12 +7615,12 @@
         <v>45</v>
       </c>
       <c r="Q86" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="87" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B87" s="3" t="s">
         <v>27</v>
@@ -7580,7 +7629,7 @@
         <v>1</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E87" s="3">
         <v>23</v>
@@ -7615,12 +7664,12 @@
         <v>20</v>
       </c>
       <c r="Q87" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="88" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="9" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B88" s="3" t="s">
         <v>43</v>
@@ -7629,7 +7678,7 @@
         <v>1</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E88" s="3">
         <v>0</v>
@@ -7664,18 +7713,18 @@
         <v>45</v>
       </c>
       <c r="Q88" s="3" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="89" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="22" t="s">
         <v>286</v>
-      </c>
-    </row>
-    <row r="89" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="7" t="s">
-        <v>287</v>
       </c>
       <c r="B89" s="3" t="s">
         <v>23</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E89" s="3">
         <v>19</v>
@@ -7697,22 +7746,23 @@
         <v>0</v>
       </c>
       <c r="L89" s="4">
-        <v>65</v>
+        <f>65+2.5</f>
+        <v>67.5</v>
       </c>
       <c r="M89" s="5">
         <v>0</v>
       </c>
       <c r="N89" s="5">
         <f t="shared" si="2"/>
-        <v>-2.5</v>
+        <v>0</v>
       </c>
       <c r="Q89" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="90" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B90" s="3" t="s">
         <v>31</v>
@@ -7721,7 +7771,7 @@
         <v>1</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E90" s="3">
         <v>23</v>
@@ -7758,12 +7808,12 @@
         <v>20</v>
       </c>
       <c r="Q90" s="3" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="91" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="22" t="s">
         <v>292</v>
-      </c>
-    </row>
-    <row r="91" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="7" t="s">
-        <v>293</v>
       </c>
       <c r="B91" s="3" t="s">
         <v>51</v>
@@ -7772,7 +7822,7 @@
         <v>1</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E91" s="3">
         <v>21</v>
@@ -7794,28 +7844,28 @@
         <v>0</v>
       </c>
       <c r="L91" s="4">
-        <v>0</v>
+        <v>22.5</v>
       </c>
       <c r="M91" s="5">
         <v>42.5</v>
       </c>
       <c r="N91" s="5">
         <f t="shared" si="2"/>
-        <v>-22.5</v>
+        <v>0</v>
       </c>
       <c r="Q91" s="3" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="92" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="22" t="s">
         <v>295</v>
-      </c>
-    </row>
-    <row r="92" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="7" t="s">
-        <v>296</v>
       </c>
       <c r="B92" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E92" s="3">
         <v>0</v>
@@ -7839,7 +7889,7 @@
       <c r="L92" s="4">
         <v>21</v>
       </c>
-      <c r="M92" s="21">
+      <c r="M92" s="20">
         <v>0</v>
       </c>
       <c r="N92" s="5">
@@ -7847,18 +7897,18 @@
         <v>0</v>
       </c>
       <c r="Q92" s="3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="93" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="9" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B93" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E93" s="3">
         <v>0</v>
@@ -7893,12 +7943,12 @@
         <v>45</v>
       </c>
       <c r="Q93" s="3" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="94" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="22" t="s">
         <v>301</v>
-      </c>
-    </row>
-    <row r="94" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="7" t="s">
-        <v>302</v>
       </c>
       <c r="B94" s="3" t="s">
         <v>43</v>
@@ -7907,7 +7957,7 @@
         <v>1</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E94" s="3">
         <v>2</v>
@@ -7931,23 +7981,23 @@
         <v>0</v>
       </c>
       <c r="L94" s="4">
-        <f>42-2</f>
-        <v>40</v>
+        <f>42-2+4</f>
+        <v>44</v>
       </c>
       <c r="M94" s="5">
         <v>0</v>
       </c>
       <c r="N94" s="5">
         <f t="shared" si="2"/>
-        <v>-4</v>
+        <v>0</v>
       </c>
       <c r="Q94" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="95" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B95" s="3" t="s">
         <v>31</v>
@@ -7956,7 +8006,7 @@
         <v>1</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E95" s="3">
         <v>0</v>
@@ -7997,12 +8047,12 @@
         <v>173</v>
       </c>
       <c r="Q95" s="3" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="96" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B96" s="3" t="s">
         <v>17</v>
@@ -8011,7 +8061,7 @@
         <v>1</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E96" s="3">
         <v>0</v>
@@ -8048,12 +8098,12 @@
         <v>20</v>
       </c>
       <c r="Q96" s="3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="97" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B97" s="3" t="s">
         <v>17</v>
@@ -8062,7 +8112,7 @@
         <v>1</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E97" s="3">
         <v>0</v>
@@ -8100,15 +8150,15 @@
         <v>20</v>
       </c>
       <c r="P97" s="16" t="s">
+        <v>312</v>
+      </c>
+      <c r="Q97" s="3" t="s">
         <v>313</v>
-      </c>
-      <c r="Q97" s="3" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="98" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B98" s="3" t="s">
         <v>55</v>
@@ -8117,7 +8167,7 @@
         <v>1</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E98" s="3">
         <v>0</v>
@@ -8152,12 +8202,12 @@
         <v>20</v>
       </c>
       <c r="Q98" s="3" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="99" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B99" s="3" t="s">
         <v>17</v>
@@ -8166,7 +8216,7 @@
         <v>1</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E99" s="3">
         <v>23</v>
@@ -8203,18 +8253,18 @@
         <v>20</v>
       </c>
       <c r="Q99" s="3" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="100" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="22" t="s">
         <v>320</v>
-      </c>
-    </row>
-    <row r="100" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="7" t="s">
-        <v>321</v>
       </c>
       <c r="B100" s="3" t="s">
         <v>43</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E100" s="3">
         <v>0</v>
@@ -8233,7 +8283,7 @@
       </c>
       <c r="J100" s="4"/>
       <c r="K100" s="4">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="L100" s="4">
         <v>0</v>
@@ -8243,15 +8293,15 @@
       </c>
       <c r="N100" s="5">
         <f t="shared" si="2"/>
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="Q100" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="101" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="9" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B101" s="3" t="s">
         <v>23</v>
@@ -8260,7 +8310,7 @@
         <v>1</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E101" s="3">
         <v>0</v>
@@ -8295,12 +8345,12 @@
         <v>45</v>
       </c>
       <c r="Q101" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="102" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B102" s="3" t="s">
         <v>17</v>
@@ -8309,7 +8359,7 @@
         <v>1</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E102" s="3">
         <v>17</v>
@@ -8347,12 +8397,12 @@
         <v>173</v>
       </c>
       <c r="Q102" s="3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="103" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B103" s="3" t="s">
         <v>23</v>
@@ -8361,7 +8411,7 @@
         <v>1</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E103" s="3">
         <v>0</v>
@@ -8375,7 +8425,7 @@
       <c r="H103" s="4">
         <v>0</v>
       </c>
-      <c r="I103" s="18" t="s">
+      <c r="I103" s="17" t="s">
         <v>19</v>
       </c>
       <c r="J103" s="4">
@@ -8401,12 +8451,12 @@
         <v>173</v>
       </c>
       <c r="Q103" s="3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="104" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B104" s="3" t="s">
         <v>23</v>
@@ -8415,7 +8465,7 @@
         <v>1</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E104" s="3">
         <v>18</v>
@@ -8429,7 +8479,7 @@
       <c r="H104" s="4">
         <v>0</v>
       </c>
-      <c r="I104" s="18" t="s">
+      <c r="I104" s="17" t="s">
         <v>19</v>
       </c>
       <c r="J104" s="4"/>
@@ -8450,20 +8500,20 @@
         <v>20</v>
       </c>
       <c r="Q104" s="3" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="105" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="22" t="s">
         <v>335</v>
-      </c>
-    </row>
-    <row r="105" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="7" t="s">
-        <v>336</v>
       </c>
       <c r="B105" s="3" t="s">
         <v>51</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>337</v>
-      </c>
-      <c r="E105" s="22">
+        <v>336</v>
+      </c>
+      <c r="E105" s="21">
         <v>8</v>
       </c>
       <c r="F105" s="3">
@@ -8483,29 +8533,30 @@
         <v>0</v>
       </c>
       <c r="L105" s="4">
-        <f>12+20</f>
-        <v>32</v>
+        <f>20-12+8</f>
+        <v>16</v>
       </c>
       <c r="M105" s="5">
         <v>0</v>
       </c>
       <c r="N105" s="5">
         <f t="shared" si="2"/>
-        <v>16</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="O105" s="23"/>
       <c r="Q105" s="3" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="106" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="22" t="s">
         <v>338</v>
-      </c>
-    </row>
-    <row r="106" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="7" t="s">
-        <v>339</v>
       </c>
       <c r="B106" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E106" s="3">
         <v>2</v>
@@ -8537,12 +8588,12 @@
         <v>0</v>
       </c>
       <c r="Q106" s="3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="107" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B107" s="3" t="s">
         <v>17</v>
@@ -8551,7 +8602,7 @@
         <v>1</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E107" s="3">
         <v>0</v>
@@ -8586,18 +8637,18 @@
         <v>20</v>
       </c>
       <c r="Q107" s="3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="108" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B108" s="3" t="s">
         <v>23</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E108" s="3">
         <v>19</v>
@@ -8611,7 +8662,7 @@
       <c r="H108" s="4">
         <v>0</v>
       </c>
-      <c r="I108" s="18" t="s">
+      <c r="I108" s="17" t="s">
         <v>19</v>
       </c>
       <c r="J108" s="4"/>
@@ -8632,12 +8683,12 @@
         <v>20</v>
       </c>
       <c r="Q108" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="109" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B109" s="3" t="s">
         <v>31</v>
@@ -8646,7 +8697,7 @@
         <v>1</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E109" s="3">
         <v>0</v>
@@ -8681,18 +8732,18 @@
         <v>20</v>
       </c>
       <c r="Q109" s="3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="110" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="7" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B110" s="3" t="s">
         <v>55</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E110" s="3">
         <v>23</v>
@@ -8723,19 +8774,20 @@
         <f t="shared" si="2"/>
         <v>-1</v>
       </c>
+      <c r="O110" s="24"/>
       <c r="Q110" s="3" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="111" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="22" t="s">
         <v>352</v>
-      </c>
-    </row>
-    <row r="111" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="7" t="s">
-        <v>353</v>
       </c>
       <c r="B111" s="3" t="s">
         <v>23</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E111" s="3">
         <v>18</v>
@@ -8757,22 +8809,22 @@
         <v>0</v>
       </c>
       <c r="L111" s="4">
-        <v>0</v>
-      </c>
-      <c r="M111" s="21">
+        <v>45</v>
+      </c>
+      <c r="M111" s="20">
         <v>0</v>
       </c>
       <c r="N111" s="5">
         <f t="shared" si="2"/>
-        <v>-45</v>
+        <v>0</v>
       </c>
       <c r="Q111" s="3" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="112" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B112" s="3" t="s">
         <v>17</v>
@@ -8781,7 +8833,7 @@
         <v>1</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E112" s="3">
         <v>23</v>
@@ -8816,18 +8868,18 @@
         <v>20</v>
       </c>
       <c r="Q112" s="3" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="113" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="22" t="s">
         <v>358</v>
-      </c>
-    </row>
-    <row r="113" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="7" t="s">
-        <v>359</v>
       </c>
       <c r="B113" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E113" s="3">
         <v>0</v>
@@ -8846,7 +8898,7 @@
       </c>
       <c r="J113" s="4"/>
       <c r="K113" s="4">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="L113" s="4">
         <v>0</v>
@@ -8856,21 +8908,21 @@
       </c>
       <c r="N113" s="5">
         <f t="shared" si="2"/>
-        <v>-45</v>
+        <v>0</v>
       </c>
       <c r="Q113" s="3" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="114" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="9" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B114" s="3" t="s">
         <v>55</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E114" s="3">
         <v>0</v>
@@ -8905,18 +8957,18 @@
         <v>45</v>
       </c>
       <c r="Q114" s="3" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="115" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="22" t="s">
         <v>364</v>
-      </c>
-    </row>
-    <row r="115" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="7" t="s">
-        <v>365</v>
       </c>
       <c r="B115" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E115" s="3">
         <v>22</v>
@@ -8935,7 +8987,7 @@
       </c>
       <c r="J115" s="4"/>
       <c r="K115" s="4">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="L115" s="4">
         <v>0</v>
@@ -8945,21 +8997,21 @@
       </c>
       <c r="N115" s="5">
         <f t="shared" si="2"/>
-        <v>-65</v>
+        <v>0</v>
       </c>
       <c r="Q115" s="3" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="116" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B116" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E116" s="3">
         <v>0</v>
@@ -8998,12 +9050,12 @@
         <v>173</v>
       </c>
       <c r="Q116" s="3" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="117" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="22" t="s">
         <v>370</v>
-      </c>
-    </row>
-    <row r="117" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="7" t="s">
-        <v>371</v>
       </c>
       <c r="B117" s="3" t="s">
         <v>51</v>
@@ -9012,7 +9064,7 @@
         <v>1</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E117" s="3">
         <v>0</v>
@@ -9036,29 +9088,29 @@
         <v>0</v>
       </c>
       <c r="L117" s="4">
-        <f>-7.5+32.5</f>
-        <v>25</v>
+        <f>-7.5+32.5+15</f>
+        <v>40</v>
       </c>
       <c r="M117" s="5">
         <v>0</v>
       </c>
       <c r="N117" s="5">
         <f t="shared" si="2"/>
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="Q117" s="3" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="118" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="7" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B118" s="3" t="s">
         <v>23</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E118" s="3">
         <v>0</v>
@@ -9090,12 +9142,12 @@
         <v>-22.5</v>
       </c>
       <c r="Q118" s="3" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="119" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B119" s="3" t="s">
         <v>17</v>
@@ -9104,7 +9156,7 @@
         <v>1</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E119" s="3">
         <v>19</v>
@@ -9142,12 +9194,12 @@
         <v>20</v>
       </c>
       <c r="Q119" s="3" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="120" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B120" s="3" t="s">
         <v>55</v>
@@ -9156,7 +9208,7 @@
         <v>1</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E120" s="3">
         <v>0</v>
@@ -9194,18 +9246,18 @@
         <v>173</v>
       </c>
       <c r="Q120" s="3" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="121" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="9" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B121" s="3" t="s">
         <v>43</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E121" s="3">
         <v>0</v>
@@ -9240,18 +9292,18 @@
         <v>45</v>
       </c>
       <c r="Q121" s="3" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="122" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="7" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B122" s="3" t="s">
         <v>43</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E122" s="3">
         <v>22</v>
@@ -9286,15 +9338,15 @@
         <v>20</v>
       </c>
       <c r="P122" s="8" t="s">
+        <v>387</v>
+      </c>
+      <c r="Q122" s="3" t="s">
         <v>388</v>
-      </c>
-      <c r="Q122" s="3" t="s">
-        <v>389</v>
       </c>
     </row>
     <row r="123" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B123" s="3" t="s">
         <v>17</v>
@@ -9303,7 +9355,7 @@
         <v>1</v>
       </c>
       <c r="D123" s="3" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="E123" s="3">
         <v>0</v>
@@ -9338,12 +9390,12 @@
         <v>20</v>
       </c>
       <c r="Q123" s="3" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="124" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B124" s="3" t="s">
         <v>27</v>
@@ -9352,7 +9404,7 @@
         <v>1</v>
       </c>
       <c r="D124" s="3" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E124" s="3">
         <v>23</v>
@@ -9390,12 +9442,12 @@
         <v>20</v>
       </c>
       <c r="Q124" s="3" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="125" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B125" s="3" t="s">
         <v>27</v>
@@ -9404,7 +9456,7 @@
         <v>1</v>
       </c>
       <c r="D125" s="3" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="E125" s="3">
         <v>0</v>
@@ -9439,12 +9491,12 @@
         <v>20</v>
       </c>
       <c r="Q125" s="3" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="126" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B126" s="3" t="s">
         <v>27</v>
@@ -9453,7 +9505,7 @@
         <v>1</v>
       </c>
       <c r="D126" s="3" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E126" s="3">
         <v>23</v>
@@ -9488,12 +9540,12 @@
         <v>20</v>
       </c>
       <c r="Q126" s="3" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="127" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A127" s="22" t="s">
         <v>401</v>
-      </c>
-    </row>
-    <row r="127" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="7" t="s">
-        <v>402</v>
       </c>
       <c r="B127" s="3" t="s">
         <v>51</v>
@@ -9526,23 +9578,23 @@
         <v>0</v>
       </c>
       <c r="L127" s="4">
-        <f>72-2</f>
-        <v>70</v>
+        <f>72-2+6</f>
+        <v>76</v>
       </c>
       <c r="M127" s="5">
         <v>0</v>
       </c>
       <c r="N127" s="5">
         <f t="shared" si="2"/>
-        <v>-6</v>
+        <v>0</v>
       </c>
       <c r="Q127" s="3" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="128" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B128" s="3" t="s">
         <v>55</v>
@@ -9551,7 +9603,7 @@
         <v>1</v>
       </c>
       <c r="D128" s="3" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E128" s="3">
         <v>0</v>
@@ -9591,12 +9643,12 @@
         <v>37</v>
       </c>
       <c r="Q128" s="3" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="129" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B129" s="3" t="s">
         <v>27</v>
@@ -9605,7 +9657,7 @@
         <v>1</v>
       </c>
       <c r="D129" s="3" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="E129" s="3">
         <v>0</v>
@@ -9640,18 +9692,18 @@
         <v>20</v>
       </c>
       <c r="Q129" s="3" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="130" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="22" t="s">
         <v>409</v>
-      </c>
-    </row>
-    <row r="130" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="7" t="s">
-        <v>410</v>
       </c>
       <c r="B130" s="3" t="s">
         <v>23</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="E130" s="3">
         <v>0</v>
@@ -9673,22 +9725,22 @@
         <v>0</v>
       </c>
       <c r="L130" s="4">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="M130" s="5">
         <v>0</v>
       </c>
       <c r="N130" s="5">
         <f t="shared" si="2"/>
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="Q130" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="131" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B131" s="3" t="s">
         <v>55</v>
@@ -9697,7 +9749,7 @@
         <v>1</v>
       </c>
       <c r="D131" s="3" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E131" s="3">
         <v>0</v>
@@ -9734,12 +9786,12 @@
         <v>20</v>
       </c>
       <c r="Q131" s="3" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="132" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B132" s="3" t="s">
         <v>17</v>
@@ -9748,7 +9800,7 @@
         <v>1</v>
       </c>
       <c r="D132" s="3" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E132" s="3">
         <v>5</v>
@@ -9783,21 +9835,21 @@
         <v>20</v>
       </c>
       <c r="P132" s="16" t="s">
+        <v>417</v>
+      </c>
+      <c r="Q132" s="3" t="s">
         <v>418</v>
-      </c>
-      <c r="Q132" s="3" t="s">
-        <v>419</v>
       </c>
     </row>
     <row r="133" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="7" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B133" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D133" s="3" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E133" s="3">
         <v>0</v>
@@ -9829,13 +9881,14 @@
         <f t="shared" si="2"/>
         <v>-2.5</v>
       </c>
+      <c r="O133" s="24"/>
       <c r="Q133" s="3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="134" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B134" s="3" t="s">
         <v>23</v>
@@ -9844,7 +9897,7 @@
         <v>1</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E134" s="3">
         <v>0</v>
@@ -9858,7 +9911,7 @@
       <c r="H134" s="4">
         <v>0</v>
       </c>
-      <c r="I134" s="18" t="s">
+      <c r="I134" s="17" t="s">
         <v>19</v>
       </c>
       <c r="J134" s="4">
@@ -9881,12 +9934,12 @@
         <v>20</v>
       </c>
       <c r="Q134" s="3" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="135" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B135" s="3" t="s">
         <v>51</v>
@@ -9895,7 +9948,7 @@
         <v>1</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="E135" s="3">
         <v>0</v>
@@ -9930,12 +9983,12 @@
         <v>20</v>
       </c>
       <c r="Q135" s="3" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="136" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A136" s="22" t="s">
         <v>428</v>
-      </c>
-    </row>
-    <row r="136" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="7" t="s">
-        <v>429</v>
       </c>
       <c r="B136" s="3" t="s">
         <v>27</v>
@@ -9944,7 +9997,7 @@
         <v>1</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E136" s="3">
         <v>1</v>
@@ -9968,23 +10021,23 @@
         <v>0</v>
       </c>
       <c r="L136" s="4">
-        <f>29-4</f>
-        <v>25</v>
+        <f>29-4+2</f>
+        <v>27</v>
       </c>
       <c r="M136" s="5">
         <v>0</v>
       </c>
       <c r="N136" s="5">
         <f t="shared" si="2"/>
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="Q136" s="3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="137" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B137" s="3" t="s">
         <v>27</v>
@@ -9993,7 +10046,7 @@
         <v>1</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="E137" s="3">
         <v>0</v>
@@ -10030,12 +10083,12 @@
         <v>20</v>
       </c>
       <c r="Q137" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="138" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B138" s="3" t="s">
         <v>43</v>
@@ -10044,7 +10097,7 @@
         <v>1</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="E138" s="3">
         <v>0</v>
@@ -10085,12 +10138,12 @@
         <v>85</v>
       </c>
       <c r="Q138" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="139" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="7" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B139" s="3" t="s">
         <v>31</v>
@@ -10099,7 +10152,7 @@
         <v>1</v>
       </c>
       <c r="D139" s="3" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E139" s="3">
         <v>3</v>
@@ -10134,15 +10187,15 @@
         <v>20</v>
       </c>
       <c r="P139" s="8" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="Q139" s="3" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="140" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B140" s="3" t="s">
         <v>27</v>
@@ -10151,7 +10204,7 @@
         <v>1</v>
       </c>
       <c r="D140" s="3" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E140" s="3">
         <v>22</v>
@@ -10186,12 +10239,12 @@
         <v>20</v>
       </c>
       <c r="Q140" s="3" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="141" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B141" s="3" t="s">
         <v>55</v>
@@ -10200,7 +10253,7 @@
         <v>1</v>
       </c>
       <c r="D141" s="3" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E141" s="3">
         <v>23</v>
@@ -10238,18 +10291,18 @@
         <v>20</v>
       </c>
       <c r="Q141" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="142" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="7" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B142" s="3" t="s">
         <v>43</v>
       </c>
       <c r="D142" s="3" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E142" s="3">
         <v>0</v>
@@ -10281,18 +10334,18 @@
         <v>-22.5</v>
       </c>
       <c r="Q142" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="143" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="7" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B143" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D143" s="3" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="E143" s="3">
         <v>0</v>
@@ -10323,19 +10376,20 @@
         <f t="shared" si="2"/>
         <v>-22.5</v>
       </c>
+      <c r="O143" s="24"/>
       <c r="Q143" s="3" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="144" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="9" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B144" s="3" t="s">
         <v>43</v>
       </c>
       <c r="D144" s="3" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="E144" s="3">
         <v>0</v>
@@ -10370,18 +10424,18 @@
         <v>45</v>
       </c>
       <c r="Q144" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="145" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="9" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B145" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D145" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E145" s="3">
         <v>0</v>
@@ -10416,7 +10470,7 @@
         <v>45</v>
       </c>
       <c r="Q145" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="146" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>